<commit_message>
update manifests, date: 2021-06-17
</commit_message>
<xml_diff>
--- a/manifests - Copy/Experiment_Manifest.xlsx
+++ b/manifests - Copy/Experiment_Manifest.xlsx
@@ -398,8 +398,8 @@
   </sheetPr>
   <dimension ref="A1:O10001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="46" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:O153"/>
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -415,8 +415,7 @@
     <col width="10.1796875" bestFit="1" customWidth="1" style="2" min="9" max="9"/>
     <col width="21.453125" bestFit="1" customWidth="1" style="2" min="10" max="10"/>
     <col width="19.08984375" bestFit="1" customWidth="1" style="2" min="11" max="11"/>
-    <col width="21.6328125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="22.453125" bestFit="1" customWidth="1" style="2" min="13" max="13"/>
+    <col width="22.453125" bestFit="1" customWidth="1" style="2" min="12" max="13"/>
     <col width="18.6328125" bestFit="1" customWidth="1" style="2" min="14" max="14"/>
   </cols>
   <sheetData>
@@ -433,12 +432,12 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>#subfolder_name</t>
+          <t>#subfolder</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>#parent_folder_name</t>
+          <t>#parent_folder</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -826,7 +825,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -894,7 +892,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -962,7 +959,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1030,7 +1026,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1098,7 +1093,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1166,7 +1160,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1234,7 +1227,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1302,7 +1294,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1370,7 +1361,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1438,7 +1428,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1506,7 +1495,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1574,7 +1562,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1642,7 +1629,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1710,7 +1696,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1778,7 +1763,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1846,7 +1830,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1914,7 +1897,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -1982,7 +1964,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -2050,7 +2031,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -2118,7 +2098,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -2186,7 +2165,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -2254,7 +2232,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -2322,7 +2299,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -2390,7 +2366,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -2746,7 +2721,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -2814,7 +2788,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -2882,7 +2855,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -2950,7 +2922,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -3018,7 +2989,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I38" t="inlineStr"/>
       <c r="J38" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -3086,7 +3056,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I39" t="inlineStr"/>
       <c r="J39" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -3154,7 +3123,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I40" t="inlineStr"/>
       <c r="J40" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -3222,7 +3190,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I41" t="inlineStr"/>
       <c r="J41" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -3290,7 +3257,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -3358,7 +3324,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I43" t="inlineStr"/>
       <c r="J43" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -3426,7 +3391,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I44" t="inlineStr"/>
       <c r="J44" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -3494,7 +3458,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I45" t="inlineStr"/>
       <c r="J45" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -3850,7 +3813,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I50" t="inlineStr"/>
       <c r="J50" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -3918,7 +3880,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I51" t="inlineStr"/>
       <c r="J51" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -3986,7 +3947,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I52" t="inlineStr"/>
       <c r="J52" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -4054,7 +4014,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I53" t="inlineStr"/>
       <c r="J53" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -4122,7 +4081,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I54" t="inlineStr"/>
       <c r="J54" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -4190,7 +4148,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I55" t="inlineStr"/>
       <c r="J55" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -4258,7 +4215,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I56" t="inlineStr"/>
       <c r="J56" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -4326,7 +4282,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I57" t="inlineStr"/>
       <c r="J57" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -4394,7 +4349,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I58" t="inlineStr"/>
       <c r="J58" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -4462,7 +4416,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I59" t="inlineStr"/>
       <c r="J59" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -4530,7 +4483,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I60" t="inlineStr"/>
       <c r="J60" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -4598,7 +4550,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I61" t="inlineStr"/>
       <c r="J61" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -4954,7 +4905,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I66" t="inlineStr"/>
       <c r="J66" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -5022,7 +4972,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I67" t="inlineStr"/>
       <c r="J67" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -5090,7 +5039,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I68" t="inlineStr"/>
       <c r="J68" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -5158,7 +5106,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I69" t="inlineStr"/>
       <c r="J69" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -5226,7 +5173,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I70" t="inlineStr"/>
       <c r="J70" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -5294,7 +5240,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I71" t="inlineStr"/>
       <c r="J71" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -5362,7 +5307,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I72" t="inlineStr"/>
       <c r="J72" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -5430,7 +5374,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I73" t="inlineStr"/>
       <c r="J73" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -5498,7 +5441,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I74" t="inlineStr"/>
       <c r="J74" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -5566,7 +5508,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I75" t="inlineStr"/>
       <c r="J75" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -5634,7 +5575,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I76" t="inlineStr"/>
       <c r="J76" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -5702,7 +5642,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I77" t="inlineStr"/>
       <c r="J77" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -6058,7 +5997,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I82" t="inlineStr"/>
       <c r="J82" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -6126,7 +6064,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I83" t="inlineStr"/>
       <c r="J83" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -6194,7 +6131,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I84" t="inlineStr"/>
       <c r="J84" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -6262,7 +6198,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I85" t="inlineStr"/>
       <c r="J85" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -6330,7 +6265,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I86" t="inlineStr"/>
       <c r="J86" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -6398,7 +6332,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I87" t="inlineStr"/>
       <c r="J87" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -6466,7 +6399,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I88" t="inlineStr"/>
       <c r="J88" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -6534,7 +6466,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I89" t="inlineStr"/>
       <c r="J89" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -6602,7 +6533,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I90" t="inlineStr"/>
       <c r="J90" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -6670,7 +6600,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I91" t="inlineStr"/>
       <c r="J91" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -6738,7 +6667,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I92" t="inlineStr"/>
       <c r="J92" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -6806,7 +6734,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I93" t="inlineStr"/>
       <c r="J93" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -7162,7 +7089,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I98" t="inlineStr"/>
       <c r="J98" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -7230,7 +7156,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I99" t="inlineStr"/>
       <c r="J99" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -7298,7 +7223,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I100" t="inlineStr"/>
       <c r="J100" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -7366,7 +7290,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I101" t="inlineStr"/>
       <c r="J101" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -7434,7 +7357,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I102" t="inlineStr"/>
       <c r="J102" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -7502,7 +7424,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I103" t="inlineStr"/>
       <c r="J103" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -7570,7 +7491,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I104" t="inlineStr"/>
       <c r="J104" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -7638,7 +7558,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I105" t="inlineStr"/>
       <c r="J105" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -7706,7 +7625,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I106" t="inlineStr"/>
       <c r="J106" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -7774,7 +7692,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I107" t="inlineStr"/>
       <c r="J107" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -7842,7 +7759,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I108" t="inlineStr"/>
       <c r="J108" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -7910,7 +7826,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I109" t="inlineStr"/>
       <c r="J109" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -8266,7 +8181,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I114" t="inlineStr"/>
       <c r="J114" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -8334,7 +8248,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I115" t="inlineStr"/>
       <c r="J115" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -8402,7 +8315,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I116" t="inlineStr"/>
       <c r="J116" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -8470,7 +8382,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I117" t="inlineStr"/>
       <c r="J117" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -8538,7 +8449,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I118" t="inlineStr"/>
       <c r="J118" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -8606,7 +8516,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I119" t="inlineStr"/>
       <c r="J119" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -8674,7 +8583,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I120" t="inlineStr"/>
       <c r="J120" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -8742,7 +8650,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I121" t="inlineStr"/>
       <c r="J121" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -8810,7 +8717,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I122" t="inlineStr"/>
       <c r="J122" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -8878,7 +8784,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I123" t="inlineStr"/>
       <c r="J123" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -8946,7 +8851,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I124" t="inlineStr"/>
       <c r="J124" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -9014,7 +8918,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I125" t="inlineStr"/>
       <c r="J125" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -9370,7 +9273,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I130" t="inlineStr"/>
       <c r="J130" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -9438,7 +9340,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I131" t="inlineStr"/>
       <c r="J131" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -9506,7 +9407,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I132" t="inlineStr"/>
       <c r="J132" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -9574,7 +9474,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I133" t="inlineStr"/>
       <c r="J133" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -9642,7 +9541,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I134" t="inlineStr"/>
       <c r="J134" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -9710,7 +9608,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I135" t="inlineStr"/>
       <c r="J135" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -9778,7 +9675,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I136" t="inlineStr"/>
       <c r="J136" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -9846,7 +9742,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I137" t="inlineStr"/>
       <c r="J137" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -9914,7 +9809,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I138" t="inlineStr"/>
       <c r="J138" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -9982,7 +9876,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I139" t="inlineStr"/>
       <c r="J139" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -10050,7 +9943,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I140" t="inlineStr"/>
       <c r="J140" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -10118,7 +10010,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I141" t="inlineStr"/>
       <c r="J141" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -10474,7 +10365,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I146" t="inlineStr"/>
       <c r="J146" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -10542,7 +10432,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I147" t="inlineStr"/>
       <c r="J147" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -10610,7 +10499,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I148" t="inlineStr"/>
       <c r="J148" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -10678,7 +10566,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I149" t="inlineStr"/>
       <c r="J149" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -10746,7 +10633,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I150" t="inlineStr"/>
       <c r="J150" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -10814,7 +10700,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I151" t="inlineStr"/>
       <c r="J151" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -10882,7 +10767,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I152" t="inlineStr"/>
       <c r="J152" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -10950,7 +10834,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I153" t="inlineStr"/>
       <c r="J153" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -11018,7 +10901,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I154" t="inlineStr"/>
       <c r="J154" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -11086,7 +10968,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I155" t="inlineStr"/>
       <c r="J155" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -11154,7 +11035,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I156" t="inlineStr"/>
       <c r="J156" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -11222,7 +11102,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I157" t="inlineStr"/>
       <c r="J157" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -11578,7 +11457,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I162" t="inlineStr"/>
       <c r="J162" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -11646,7 +11524,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I163" t="inlineStr"/>
       <c r="J163" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -11714,7 +11591,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I164" t="inlineStr"/>
       <c r="J164" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -11782,7 +11658,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I165" t="inlineStr"/>
       <c r="J165" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -11850,7 +11725,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I166" t="inlineStr"/>
       <c r="J166" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -11918,7 +11792,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I167" t="inlineStr"/>
       <c r="J167" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -11986,7 +11859,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I168" t="inlineStr"/>
       <c r="J168" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -12054,7 +11926,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I169" t="inlineStr"/>
       <c r="J169" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -12122,7 +11993,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I170" t="inlineStr"/>
       <c r="J170" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -12190,7 +12060,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I171" t="inlineStr"/>
       <c r="J171" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -12258,7 +12127,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I172" t="inlineStr"/>
       <c r="J172" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -12326,7 +12194,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I173" t="inlineStr"/>
       <c r="J173" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -12682,7 +12549,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I178" t="inlineStr"/>
       <c r="J178" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -12750,7 +12616,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I179" t="inlineStr"/>
       <c r="J179" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -12818,7 +12683,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I180" t="inlineStr"/>
       <c r="J180" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -12886,7 +12750,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I181" t="inlineStr"/>
       <c r="J181" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -12954,7 +12817,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I182" t="inlineStr"/>
       <c r="J182" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -13022,7 +12884,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I183" t="inlineStr"/>
       <c r="J183" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -13090,7 +12951,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I184" t="inlineStr"/>
       <c r="J184" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -13158,7 +13018,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I185" t="inlineStr"/>
       <c r="J185" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -13226,7 +13085,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I186" t="inlineStr"/>
       <c r="J186" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -13294,7 +13152,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I187" t="inlineStr"/>
       <c r="J187" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -13362,7 +13219,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I188" t="inlineStr"/>
       <c r="J188" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -13430,7 +13286,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I189" t="inlineStr"/>
       <c r="J189" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -13786,7 +13641,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I194" t="inlineStr"/>
       <c r="J194" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -13854,7 +13708,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I195" t="inlineStr"/>
       <c r="J195" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -13922,7 +13775,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I196" t="inlineStr"/>
       <c r="J196" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -13990,7 +13842,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I197" t="inlineStr"/>
       <c r="J197" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -14058,7 +13909,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I198" t="inlineStr"/>
       <c r="J198" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -14126,7 +13976,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I199" t="inlineStr"/>
       <c r="J199" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -14194,7 +14043,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I200" t="inlineStr"/>
       <c r="J200" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -14262,7 +14110,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I201" t="inlineStr"/>
       <c r="J201" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -14330,7 +14177,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I202" t="inlineStr"/>
       <c r="J202" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -14398,7 +14244,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I203" t="inlineStr"/>
       <c r="J203" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -14466,7 +14311,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I204" t="inlineStr"/>
       <c r="J204" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -14534,7 +14378,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I205" t="inlineStr"/>
       <c r="J205" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -14890,7 +14733,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I210" t="inlineStr"/>
       <c r="J210" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -14958,7 +14800,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I211" t="inlineStr"/>
       <c r="J211" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -15026,7 +14867,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I212" t="inlineStr"/>
       <c r="J212" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -15094,7 +14934,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I213" t="inlineStr"/>
       <c r="J213" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -15162,7 +15001,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I214" t="inlineStr"/>
       <c r="J214" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -15230,7 +15068,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I215" t="inlineStr"/>
       <c r="J215" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -15298,7 +15135,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I216" t="inlineStr"/>
       <c r="J216" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -15366,7 +15202,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I217" t="inlineStr"/>
       <c r="J217" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -15434,7 +15269,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I218" t="inlineStr"/>
       <c r="J218" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -15502,7 +15336,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I219" t="inlineStr"/>
       <c r="J219" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -15570,7 +15403,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I220" t="inlineStr"/>
       <c r="J220" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -15638,7 +15470,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I221" t="inlineStr"/>
       <c r="J221" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -15994,7 +15825,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I226" t="inlineStr"/>
       <c r="J226" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -16062,7 +15892,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I227" t="inlineStr"/>
       <c r="J227" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -16130,7 +15959,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I228" t="inlineStr"/>
       <c r="J228" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -16198,7 +16026,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I229" t="inlineStr"/>
       <c r="J229" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -16266,7 +16093,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I230" t="inlineStr"/>
       <c r="J230" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -16334,7 +16160,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I231" t="inlineStr"/>
       <c r="J231" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -16402,7 +16227,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I232" t="inlineStr"/>
       <c r="J232" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -16470,7 +16294,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I233" t="inlineStr"/>
       <c r="J233" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -16538,7 +16361,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I234" t="inlineStr"/>
       <c r="J234" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -16606,7 +16428,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I235" t="inlineStr"/>
       <c r="J235" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -16674,7 +16495,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I236" t="inlineStr"/>
       <c r="J236" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -16742,7 +16562,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I237" t="inlineStr"/>
       <c r="J237" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -17098,7 +16917,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I242" t="inlineStr"/>
       <c r="J242" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -17166,7 +16984,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I243" t="inlineStr"/>
       <c r="J243" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -17234,7 +17051,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I244" t="inlineStr"/>
       <c r="J244" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -17302,7 +17118,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I245" t="inlineStr"/>
       <c r="J245" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -17370,7 +17185,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I246" t="inlineStr"/>
       <c r="J246" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -17438,7 +17252,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I247" t="inlineStr"/>
       <c r="J247" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -17506,7 +17319,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I248" t="inlineStr"/>
       <c r="J248" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -17574,7 +17386,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I249" t="inlineStr"/>
       <c r="J249" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -17642,7 +17453,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I250" t="inlineStr"/>
       <c r="J250" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -17710,7 +17520,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I251" t="inlineStr"/>
       <c r="J251" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -17778,7 +17587,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I252" t="inlineStr"/>
       <c r="J252" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -17846,7 +17654,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I253" t="inlineStr"/>
       <c r="J253" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -18202,7 +18009,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I258" t="inlineStr"/>
       <c r="J258" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -18270,7 +18076,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I259" t="inlineStr"/>
       <c r="J259" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -18338,7 +18143,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I260" t="inlineStr"/>
       <c r="J260" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -18406,7 +18210,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I261" t="inlineStr"/>
       <c r="J261" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -18474,7 +18277,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I262" t="inlineStr"/>
       <c r="J262" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -18542,7 +18344,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I263" t="inlineStr"/>
       <c r="J263" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -18610,7 +18411,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I264" t="inlineStr"/>
       <c r="J264" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -18678,7 +18478,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I265" t="inlineStr"/>
       <c r="J265" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -18746,7 +18545,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I266" t="inlineStr"/>
       <c r="J266" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -18814,7 +18612,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I267" t="inlineStr"/>
       <c r="J267" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -18882,7 +18679,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I268" t="inlineStr"/>
       <c r="J268" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -18950,7 +18746,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="I269" t="inlineStr"/>
       <c r="J269" t="inlineStr">
         <is>
           <t>None, None</t>
@@ -19266,28 +19061,620 @@
       </c>
     </row>
     <row r="274">
-      <c r="A274" s="1" t="n"/>
+      <c r="A274" s="1" t="inlineStr">
+        <is>
+          <t>e273</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>e273_4321_1_1_UnitedStoneInternational_Cleveland_OH_.jpeg</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>4321_DallasWhite_c8</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>6-16-2021_UnitedStoneInternational_Cleveland_OH</t>
+        </is>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>IMG_3070 - Copyjpeg</t>
+        </is>
+      </c>
+      <c r="F274" t="inlineStr">
+        <is>
+          <t>UnitedStoneInternational</t>
+        </is>
+      </c>
+      <c r="G274" t="inlineStr">
+        <is>
+          <t>Cleveland, OH</t>
+        </is>
+      </c>
+      <c r="H274" t="inlineStr">
+        <is>
+          <t>DallasWhite</t>
+        </is>
+      </c>
+      <c r="I274" t="inlineStr">
+        <is>
+          <t>4321</t>
+        </is>
+      </c>
+      <c r="J274" t="inlineStr">
+        <is>
+          <t>2020-07-09 14:33:40</t>
+        </is>
+      </c>
+      <c r="K274" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="L274" t="inlineStr">
+        <is>
+          <t>columns8</t>
+        </is>
+      </c>
+      <c r="M274" t="inlineStr">
+        <is>
+          <t>165.27474785372564</t>
+        </is>
+      </c>
+      <c r="N274" t="inlineStr">
+        <is>
+          <t>0.10626314137255605</t>
+        </is>
+      </c>
+      <c r="O274" t="inlineStr">
+        <is>
+          <t>(1766, 1.2229455581121895, 0.6614104882459312, 0.413381555153707, 1.2921876388374214)</t>
+        </is>
+      </c>
     </row>
     <row r="275">
-      <c r="A275" s="1" t="n"/>
+      <c r="A275" s="1" t="inlineStr">
+        <is>
+          <t>e274</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>e274_4321_1_2_UnitedStoneInternational_Cleveland_OH_.jpeg</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>4321_DallasWhite_c8</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>6-16-2021_UnitedStoneInternational_Cleveland_OH</t>
+        </is>
+      </c>
+      <c r="E275" t="inlineStr">
+        <is>
+          <t>IMG_3070jpeg</t>
+        </is>
+      </c>
+      <c r="F275" t="inlineStr">
+        <is>
+          <t>UnitedStoneInternational</t>
+        </is>
+      </c>
+      <c r="G275" t="inlineStr">
+        <is>
+          <t>Cleveland, OH</t>
+        </is>
+      </c>
+      <c r="H275" t="inlineStr">
+        <is>
+          <t>DallasWhite</t>
+        </is>
+      </c>
+      <c r="I275" t="inlineStr">
+        <is>
+          <t>4321</t>
+        </is>
+      </c>
+      <c r="J275" t="inlineStr">
+        <is>
+          <t>2020-07-09 14:33:40</t>
+        </is>
+      </c>
+      <c r="K275" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="L275" t="inlineStr">
+        <is>
+          <t>columns8</t>
+        </is>
+      </c>
+      <c r="M275" t="inlineStr">
+        <is>
+          <t>165.27474785372564</t>
+        </is>
+      </c>
+      <c r="N275" t="inlineStr">
+        <is>
+          <t>0.10626314137255605</t>
+        </is>
+      </c>
+      <c r="O275" t="inlineStr">
+        <is>
+          <t>(1766, 1.2229455581121895, 0.6614104882459312, 0.413381555153707, 1.2921876388374214)</t>
+        </is>
+      </c>
     </row>
     <row r="276">
-      <c r="A276" s="1" t="n"/>
+      <c r="A276" s="1" t="inlineStr">
+        <is>
+          <t>e275</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>e275_4321_1_3_UnitedStoneInternational_Cleveland_OH_.jpeg</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>4321_DallasWhite_c8</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>6-16-2021_UnitedStoneInternational_Cleveland_OH</t>
+        </is>
+      </c>
+      <c r="E276" t="inlineStr">
+        <is>
+          <t>IMG_3070HorFlip - Copyjpeg</t>
+        </is>
+      </c>
+      <c r="F276" t="inlineStr">
+        <is>
+          <t>UnitedStoneInternational</t>
+        </is>
+      </c>
+      <c r="G276" t="inlineStr">
+        <is>
+          <t>Cleveland, OH</t>
+        </is>
+      </c>
+      <c r="H276" t="inlineStr">
+        <is>
+          <t>DallasWhite</t>
+        </is>
+      </c>
+      <c r="I276" t="inlineStr">
+        <is>
+          <t>4321</t>
+        </is>
+      </c>
+      <c r="J276" t="inlineStr">
+        <is>
+          <t>6-16-2021</t>
+        </is>
+      </c>
+      <c r="K276" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="L276" t="inlineStr">
+        <is>
+          <t>columns8</t>
+        </is>
+      </c>
+      <c r="M276" t="inlineStr">
+        <is>
+          <t>176.2933681716365</t>
+        </is>
+      </c>
+      <c r="N276" t="inlineStr">
+        <is>
+          <t>0.10629850658417507</t>
+        </is>
+      </c>
+      <c r="O276" t="inlineStr">
+        <is>
+          <t>(1766, 1.2199003546381992, 0.6614104882459312, 0.413381555153707, 1.2678898364915758)</t>
+        </is>
+      </c>
     </row>
     <row r="277">
-      <c r="A277" s="1" t="n"/>
+      <c r="A277" s="1" t="inlineStr">
+        <is>
+          <t>e276</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>e276_4321_1_4_UnitedStoneInternational_Cleveland_OH_.jpeg</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>4321_DallasWhite_c8</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>6-16-2021_UnitedStoneInternational_Cleveland_OH</t>
+        </is>
+      </c>
+      <c r="E277" t="inlineStr">
+        <is>
+          <t>IMG_3070HorFlipjpeg</t>
+        </is>
+      </c>
+      <c r="F277" t="inlineStr">
+        <is>
+          <t>UnitedStoneInternational</t>
+        </is>
+      </c>
+      <c r="G277" t="inlineStr">
+        <is>
+          <t>Cleveland, OH</t>
+        </is>
+      </c>
+      <c r="H277" t="inlineStr">
+        <is>
+          <t>DallasWhite</t>
+        </is>
+      </c>
+      <c r="I277" t="inlineStr">
+        <is>
+          <t>4321</t>
+        </is>
+      </c>
+      <c r="J277" t="inlineStr">
+        <is>
+          <t>6-16-2021</t>
+        </is>
+      </c>
+      <c r="K277" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="L277" t="inlineStr">
+        <is>
+          <t>columns8</t>
+        </is>
+      </c>
+      <c r="M277" t="inlineStr">
+        <is>
+          <t>176.2933681716365</t>
+        </is>
+      </c>
+      <c r="N277" t="inlineStr">
+        <is>
+          <t>0.10629850658417507</t>
+        </is>
+      </c>
+      <c r="O277" t="inlineStr">
+        <is>
+          <t>(1766, 1.2199003546381992, 0.6614104882459312, 0.413381555153707, 1.2678898364915758)</t>
+        </is>
+      </c>
     </row>
     <row r="278">
-      <c r="A278" s="1" t="n"/>
+      <c r="A278" s="1" t="inlineStr">
+        <is>
+          <t>e277</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>e277_4321_1_5_UnitedStoneInternational_Cleveland_OH_.jpeg</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>4321_DallasWhite_c8</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>6-16-2021_UnitedStoneInternational_Cleveland_OH</t>
+        </is>
+      </c>
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>IMG_3070HorVertFlip - Copyjpeg</t>
+        </is>
+      </c>
+      <c r="F278" t="inlineStr">
+        <is>
+          <t>UnitedStoneInternational</t>
+        </is>
+      </c>
+      <c r="G278" t="inlineStr">
+        <is>
+          <t>Cleveland, OH</t>
+        </is>
+      </c>
+      <c r="H278" t="inlineStr">
+        <is>
+          <t>DallasWhite</t>
+        </is>
+      </c>
+      <c r="I278" t="inlineStr">
+        <is>
+          <t>4321</t>
+        </is>
+      </c>
+      <c r="J278" t="inlineStr">
+        <is>
+          <t>6-16-2021</t>
+        </is>
+      </c>
+      <c r="K278" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="L278" t="inlineStr">
+        <is>
+          <t>columns8</t>
+        </is>
+      </c>
+      <c r="M278" t="inlineStr">
+        <is>
+          <t>171.15013017929488</t>
+        </is>
+      </c>
+      <c r="N278" t="inlineStr">
+        <is>
+          <t>0.10635143177604318</t>
+        </is>
+      </c>
+      <c r="O278" t="inlineStr">
+        <is>
+          <t>(1762, 1.225678035511058, 0.6614104882459312, 0.413381555153707, 1.2904231659976855)</t>
+        </is>
+      </c>
     </row>
     <row r="279">
-      <c r="A279" s="1" t="n"/>
+      <c r="A279" s="1" t="inlineStr">
+        <is>
+          <t>e278</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>e278_4321_1_6_UnitedStoneInternational_Cleveland_OH_.jpeg</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>4321_DallasWhite_c8</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>6-16-2021_UnitedStoneInternational_Cleveland_OH</t>
+        </is>
+      </c>
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>IMG_3070HorVertFlipjpeg</t>
+        </is>
+      </c>
+      <c r="F279" t="inlineStr">
+        <is>
+          <t>UnitedStoneInternational</t>
+        </is>
+      </c>
+      <c r="G279" t="inlineStr">
+        <is>
+          <t>Cleveland, OH</t>
+        </is>
+      </c>
+      <c r="H279" t="inlineStr">
+        <is>
+          <t>DallasWhite</t>
+        </is>
+      </c>
+      <c r="I279" t="inlineStr">
+        <is>
+          <t>4321</t>
+        </is>
+      </c>
+      <c r="J279" t="inlineStr">
+        <is>
+          <t>6-16-2021</t>
+        </is>
+      </c>
+      <c r="K279" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="L279" t="inlineStr">
+        <is>
+          <t>columns8</t>
+        </is>
+      </c>
+      <c r="M279" t="inlineStr">
+        <is>
+          <t>171.15013017929488</t>
+        </is>
+      </c>
+      <c r="N279" t="inlineStr">
+        <is>
+          <t>0.10635143177604318</t>
+        </is>
+      </c>
+      <c r="O279" t="inlineStr">
+        <is>
+          <t>(1762, 1.225678035511058, 0.6614104882459312, 0.413381555153707, 1.2904231659976855)</t>
+        </is>
+      </c>
     </row>
     <row r="280">
-      <c r="A280" s="1" t="n"/>
+      <c r="A280" s="1" t="inlineStr">
+        <is>
+          <t>e279</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>e279_4321_1_7_UnitedStoneInternational_Cleveland_OH_.jpeg</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>4321_DallasWhite_c8</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>6-16-2021_UnitedStoneInternational_Cleveland_OH</t>
+        </is>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>IMG_3070VertFlip - Copyjpeg</t>
+        </is>
+      </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>UnitedStoneInternational</t>
+        </is>
+      </c>
+      <c r="G280" t="inlineStr">
+        <is>
+          <t>Cleveland, OH</t>
+        </is>
+      </c>
+      <c r="H280" t="inlineStr">
+        <is>
+          <t>DallasWhite</t>
+        </is>
+      </c>
+      <c r="I280" t="inlineStr">
+        <is>
+          <t>4321</t>
+        </is>
+      </c>
+      <c r="J280" t="inlineStr">
+        <is>
+          <t>6-16-2021</t>
+        </is>
+      </c>
+      <c r="K280" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="L280" t="inlineStr">
+        <is>
+          <t>columns8</t>
+        </is>
+      </c>
+      <c r="M280" t="inlineStr">
+        <is>
+          <t>172.45188887966015</t>
+        </is>
+      </c>
+      <c r="N280" t="inlineStr">
+        <is>
+          <t>0.10632121683796092</t>
+        </is>
+      </c>
+      <c r="O280" t="inlineStr">
+        <is>
+          <t>(1765, 1.2229526718381063, 0.6614104882459312, 0.413381555153707, 1.2822941522156464)</t>
+        </is>
+      </c>
     </row>
     <row r="281">
-      <c r="A281" s="1" t="n"/>
+      <c r="A281" s="1" t="inlineStr">
+        <is>
+          <t>e280</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>e280_4321_2_7_UnitedStoneInternational_Cleveland_OH_.jpeg</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>4321_DallasWhite_c8</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>6-16-2021_UnitedStoneInternational_Cleveland_OH</t>
+        </is>
+      </c>
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>IMG_3070VertFlipjpeg</t>
+        </is>
+      </c>
+      <c r="F281" t="inlineStr">
+        <is>
+          <t>UnitedStoneInternational</t>
+        </is>
+      </c>
+      <c r="G281" t="inlineStr">
+        <is>
+          <t>Cleveland, OH</t>
+        </is>
+      </c>
+      <c r="H281" t="inlineStr">
+        <is>
+          <t>DallasWhite</t>
+        </is>
+      </c>
+      <c r="I281" t="inlineStr">
+        <is>
+          <t>4321</t>
+        </is>
+      </c>
+      <c r="J281" t="inlineStr">
+        <is>
+          <t>6-16-2021</t>
+        </is>
+      </c>
+      <c r="K281" t="inlineStr">
+        <is>
+          <t>None, None</t>
+        </is>
+      </c>
+      <c r="L281" t="inlineStr">
+        <is>
+          <t>columns8</t>
+        </is>
+      </c>
+      <c r="M281" t="inlineStr">
+        <is>
+          <t>172.45188887966015</t>
+        </is>
+      </c>
+      <c r="N281" t="inlineStr">
+        <is>
+          <t>0.10632121683796092</t>
+        </is>
+      </c>
+      <c r="O281" t="inlineStr">
+        <is>
+          <t>(1765, 1.2229526718381063, 0.6614104882459312, 0.413381555153707, 1.2822941522156464)</t>
+        </is>
+      </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="n"/>

</xml_diff>